<commit_message>
buttons and encoder code
</commit_message>
<xml_diff>
--- a/Board Documentation/Memory Map.xlsx
+++ b/Board Documentation/Memory Map.xlsx
@@ -5,7 +5,7 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmenninger/Documents/Important/School/Caltech/Classes/EE:CS 052/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmenninger/Documents/Important/School/Caltech/Classes/EE:CS 052/EECS52/Board Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,57 +24,69 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>SRAM</t>
   </si>
   <si>
-    <t>DRAM</t>
-  </si>
-  <si>
-    <t>SD Card</t>
-  </si>
-  <si>
     <t>Buttons</t>
   </si>
   <si>
-    <t>Rotary Encoder</t>
-  </si>
-  <si>
-    <t>MP3 Decoder</t>
-  </si>
-  <si>
-    <t>Audio</t>
-  </si>
-  <si>
-    <t>Display</t>
-  </si>
-  <si>
-    <t>IDE</t>
-  </si>
-  <si>
     <t>EEROM</t>
   </si>
   <si>
-    <t>PLD</t>
-  </si>
-  <si>
     <t>Memory Map</t>
   </si>
   <si>
-    <t>MCS: 256 KB</t>
-  </si>
-  <si>
     <t>PCS: 128 B</t>
   </si>
   <si>
     <t>UCS: 256 KB</t>
   </si>
   <si>
-    <t>Unused: 261 KB</t>
-  </si>
-  <si>
     <t>LCS: 128 KB</t>
+  </si>
+  <si>
+    <t>MCS: 128 KB</t>
+  </si>
+  <si>
+    <t>PCS Map</t>
+  </si>
+  <si>
+    <t>MCS0</t>
+  </si>
+  <si>
+    <t>MCS1</t>
+  </si>
+  <si>
+    <t>MCS2</t>
+  </si>
+  <si>
+    <t>MCS3</t>
+  </si>
+  <si>
+    <t>PCS: 896 B</t>
+  </si>
+  <si>
+    <t>PCS2</t>
+  </si>
+  <si>
+    <t>PCS3</t>
+  </si>
+  <si>
+    <t>PCS4</t>
+  </si>
+  <si>
+    <t>PCS5</t>
+  </si>
+  <si>
+    <t>PCS6</t>
+  </si>
+  <si>
+    <t>Unused: ~128 KB</t>
+  </si>
+  <si>
+    <t>Rotary Encoders</t>
   </si>
 </sst>
 </file>
@@ -100,7 +112,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,8 +122,14 @@
     <fill>
       <patternFill patternType="lightGray"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="65"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -171,18 +189,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -198,9 +226,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -213,11 +238,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -496,226 +545,312 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="G7" sqref="G7:G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="4"/>
+    <col min="1" max="1" width="10.83203125" style="3"/>
     <col min="2" max="2" width="13.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="5"/>
+    <col min="3" max="3" width="10.83203125" style="4"/>
+    <col min="6" max="6" width="10.83203125" style="1"/>
+    <col min="8" max="8" width="10.83203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="str">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="F1" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="str">
         <f>"00 0000"</f>
         <v>00 0000</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="3"/>
-      <c r="B4" s="12"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="str">
+      <c r="C3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1" t="str">
+        <f>"0A 0000"</f>
+        <v>0A 0000</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="2"/>
+      <c r="B4" s="14"/>
+      <c r="G4" s="14"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" s="2"/>
+      <c r="B5" s="14"/>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="10"/>
+      <c r="G6" s="10"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="str">
         <f>"02 0000"</f>
         <v>02 0000</v>
       </c>
-      <c r="B5" s="13"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="14"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="str">
+      <c r="B7" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="str">
+        <f>"0A 0080"</f>
+        <v>0A 0080</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>20</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="11"/>
+      <c r="G8" s="19"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="11"/>
+      <c r="G9" s="19"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="13"/>
+      <c r="G10" s="20"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="str">
         <f>"04 0000"</f>
         <v>04 0000</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B8" s="6"/>
-      <c r="C8" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B9" s="6"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="str">
+      <c r="B11" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" s="1" t="str">
+        <f>"0A 0100"</f>
+        <v>0A 0100</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="5"/>
+      <c r="G12" s="14"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="5"/>
+      <c r="G13" s="14"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="5"/>
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="str">
+        <f>"06 0000"</f>
+        <v>06 0000</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="1" t="str">
+        <f>"0A 0180"</f>
+        <v>0A 0180</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="5"/>
+      <c r="G16" s="14"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="5"/>
+      <c r="G17" s="14"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="5"/>
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="str">
         <f>"08 0000"</f>
         <v>08 0000</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="5" t="s">
+      <c r="B19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F19" s="1" t="str">
+        <f>"0A 0200"</f>
+        <v>0A 0200</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="5"/>
+      <c r="G20" s="14"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="5"/>
+      <c r="G21" s="14"/>
+    </row>
+    <row r="22" spans="1:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="9"/>
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="1:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="str">
+        <f>"0A 0380"</f>
+        <v>0A 0380</v>
+      </c>
+      <c r="B23" s="17"/>
+      <c r="C23" s="4" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="str">
-        <f>"08 0080"</f>
-        <v>08 0080</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="str">
-        <f>"08 0100"</f>
-        <v>08 0100</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="F23" s="1" t="str">
+        <f>"0A 0280"</f>
+        <v>0A 0280</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H23" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="str">
-        <f>"08 0180"</f>
-        <v>08 0180</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="str">
-        <f>"08 0200"</f>
-        <v>08 0200</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="str">
-        <f>"08 0280"</f>
-        <v>08 0280</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="str">
-        <f>"08 0300"</f>
-        <v>08 0300</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="str">
-        <f>"08 0380"</f>
-        <v>08 0380</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="str">
-        <f>"08 0400"</f>
-        <v>08 0400</v>
-      </c>
-      <c r="B19" s="8"/>
-    </row>
-    <row r="20" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="9"/>
-    </row>
-    <row r="21" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="9"/>
-    </row>
-    <row r="22" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="9"/>
-      <c r="C22" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="9"/>
-    </row>
-    <row r="24" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="9"/>
-    </row>
-    <row r="25" spans="1:3" ht="20" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B25" s="10"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="str">
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="7"/>
+      <c r="C24" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="14"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="7"/>
+      <c r="G25" s="14"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="8"/>
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="str">
         <f>"0C 0000"</f>
         <v>0C 0000</v>
       </c>
-      <c r="B26" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B27" s="6"/>
-      <c r="C27" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="str">
+      <c r="B27" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F27" s="1" t="str">
+        <f>"0A 0300"</f>
+        <v>0A 0300</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="H27" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="5"/>
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="5"/>
+      <c r="G29" s="5"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B30" s="5"/>
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="5"/>
+      <c r="G31" s="16"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="5"/>
+      <c r="G32" s="16"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B33" s="5"/>
+      <c r="G33" s="16"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="str">
         <f>"0F FFFF"</f>
         <v>0F FFFF</v>
       </c>
-      <c r="B28" s="6"/>
+      <c r="B34" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="16">
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="G19:G22"/>
+    <mergeCell ref="G15:G18"/>
+    <mergeCell ref="G11:G14"/>
+    <mergeCell ref="G7:G10"/>
+    <mergeCell ref="G3:G6"/>
+    <mergeCell ref="G23:G26"/>
+    <mergeCell ref="G27:G30"/>
+    <mergeCell ref="B27:B34"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="B3:B6"/>
     <mergeCell ref="B7:B10"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="B19:B25"/>
-    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="B19:B22"/>
+    <mergeCell ref="B15:B18"/>
+    <mergeCell ref="B11:B14"/>
+    <mergeCell ref="B23:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>